<commit_message>
Updated Python model, README, and cleaned data file
</commit_message>
<xml_diff>
--- a/Cleaned_Data.xlsx
+++ b/Cleaned_Data.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\思庭\AppData\Local\Programs\Python\Python313\dataverse_files tbi Dec 2024 ML Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103D8B9E-908D-4A84-AF9F-F2EF2C2A0FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943AECED-2F60-4379-BD11-843FD3F71CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="PCS">Sheet1!$R$3:$AM$156</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -141,9 +144,6 @@
     <t>PCS 11</t>
   </si>
   <si>
-    <t>PCS12</t>
-  </si>
-  <si>
     <t>PCS 13</t>
   </si>
   <si>
@@ -198,13 +198,7 @@
     <t>MFQ 8</t>
   </si>
   <si>
-    <t>MFQ9</t>
-  </si>
-  <si>
     <t>MFQ 10</t>
-  </si>
-  <si>
-    <t>MFQ11</t>
   </si>
   <si>
     <t>MFQ 12</t>
@@ -271,6 +265,15 @@
   </si>
   <si>
     <t>MFQ 33</t>
+  </si>
+  <si>
+    <t>PCS 12</t>
+  </si>
+  <si>
+    <t>MFQ 9</t>
+  </si>
+  <si>
+    <t>MFQ 11</t>
   </si>
 </sst>
 </file>
@@ -635,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BT156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -727,136 +730,136 @@
         <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:72" x14ac:dyDescent="0.45">

</xml_diff>